<commit_message>
update, fix bug and add server launcher
</commit_message>
<xml_diff>
--- a/public/template/Data Pembayaran Komite Semester Ganjil.xlsx
+++ b/public/template/Data Pembayaran Komite Semester Ganjil.xlsx
@@ -4,13 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView activeTab="3" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView activeTab="2" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="19 kcy 3" sheetId="1" r:id="rId4"/>
-    <sheet name="27 jmy 6" sheetId="2" r:id="rId5"/>
-    <sheet name="12 MIA 2" sheetId="3" r:id="rId6"/>
-    <sheet name="04 gbk 2" sheetId="4" r:id="rId7"/>
+    <sheet name="27 jmy 6" sheetId="1" r:id="rId4"/>
+    <sheet name="12 MIA 2" sheetId="2" r:id="rId5"/>
+    <sheet name="04 gbk 2" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
@@ -18,18 +17,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
   <si>
     <t>DAFTAR PEMBAYARAN ADMINISTRASI KOMITE</t>
   </si>
   <si>
-    <t>TAHUN AJARAN 2022/2023</t>
+    <t>TAHUN AJARAN 20329</t>
   </si>
   <si>
     <t>SEMESTER GANJIL (I)</t>
   </si>
   <si>
-    <t>KELAS 19 kcy 3</t>
+    <t>KELAS 27 jmy 6</t>
   </si>
   <si>
     <t>NO</t>
@@ -62,34 +61,19 @@
     <t>DESEMBER</t>
   </si>
   <si>
-    <t>Rafi Mansur M.Ak</t>
+    <t>Silvia Nurdiyanti</t>
   </si>
   <si>
-    <t>Lunas</t>
+    <t>Rp. 0</t>
   </si>
   <si>
     <t>Belum Lunas</t>
   </si>
   <si>
-    <t>Yosef Mustofa</t>
+    <t>Siska Genta Hasanah M.Ak</t>
   </si>
   <si>
-    <t>Cayadi Harja Manullang</t>
-  </si>
-  <si>
-    <t>Jeje Saputra</t>
-  </si>
-  <si>
-    <t>Putri Isnaini</t>
-  </si>
-  <si>
-    <t>KELAS 27 jmy 6</t>
-  </si>
-  <si>
-    <t>Silvia Nurdiyanti</t>
-  </si>
-  <si>
-    <t>Siska Genta Hasanah M.Ak</t>
+    <t>Rp. 420.000</t>
   </si>
   <si>
     <t>Hudi Gloria</t>
@@ -98,58 +82,13 @@
     <t>KELAS 12 MIA 2</t>
   </si>
   <si>
-    <t>Jaswadi Lazuardi</t>
-  </si>
-  <si>
-    <t>Balijan Prayoga</t>
-  </si>
-  <si>
-    <t>Suci Yuliarti</t>
-  </si>
-  <si>
-    <t>Alika Novitasari</t>
-  </si>
-  <si>
-    <t>Aurora Suryatmi M.Kom.</t>
-  </si>
-  <si>
-    <t>Jamalia Astuti</t>
-  </si>
-  <si>
-    <t>Irma Raina Kusmawati</t>
+    <t>Yosef Mustofa</t>
   </si>
   <si>
     <t>KELAS 04 gbk 2</t>
   </si>
   <si>
-    <t>Melinda Jane Yulianti S.Sos</t>
-  </si>
-  <si>
-    <t>Paiman Simbolon</t>
-  </si>
-  <si>
-    <t>Cornelia Belinda Laksita</t>
-  </si>
-  <si>
-    <t>Kamaria Cornelia Oktaviani S.Psi</t>
-  </si>
-  <si>
-    <t>Mahesa Nugroho M.Kom.</t>
-  </si>
-  <si>
-    <t>Rp. 600.000</t>
-  </si>
-  <si>
-    <t>Lili Uyainah</t>
-  </si>
-  <si>
-    <t>Radika Saefullah</t>
-  </si>
-  <si>
-    <t>Yani Maryati</t>
-  </si>
-  <si>
-    <t>Ade Kurniawan</t>
+    <t>sadsads fe</t>
   </si>
 </sst>
 </file>
@@ -661,7 +600,7 @@
   <dimension ref="A1:P45"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" zoomScale="115" zoomScaleNormal="115" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -807,8 +746,8 @@
       <c r="B9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="20" t="s">
-        <v>15</v>
+      <c r="C9" s="21" t="s">
+        <v>18</v>
       </c>
       <c r="D9" s="21" t="s">
         <v>16</v>
@@ -835,11 +774,11 @@
         <v>3</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="20" t="s">
-        <v>15</v>
-      </c>
       <c r="D10" s="21" t="s">
         <v>16</v>
       </c>
@@ -860,62 +799,26 @@
       </c>
     </row>
     <row r="11" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A11" s="1">
-        <v>4</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="I11" s="21" t="s">
-        <v>16</v>
-      </c>
+      <c r="A11" s="1"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
     </row>
     <row r="12" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A12" s="1">
-        <v>5</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="I12" s="21" t="s">
-        <v>16</v>
-      </c>
+      <c r="A12" s="1"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
     </row>
     <row r="13" spans="1:16" customHeight="1" ht="21.9">
       <c r="A13" s="1"/>
@@ -1305,7 +1208,7 @@
   <dimension ref="A1:P45"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" zoomScale="115" zoomScaleNormal="115" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1365,7 +1268,7 @@
     </row>
     <row r="5" spans="1:16" customHeight="1" ht="15.6">
       <c r="A5" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="17"/>
     </row>
@@ -1418,10 +1321,10 @@
         <v>1</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>15</v>
+        <v>21</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>18</v>
       </c>
       <c r="D8" s="21" t="s">
         <v>16</v>
@@ -1445,63 +1348,27 @@
       <c r="O8" s="4"/>
     </row>
     <row r="9" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A9" s="1">
-        <v>2</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="I9" s="21" t="s">
-        <v>16</v>
-      </c>
+      <c r="A9" s="1"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
       <c r="M9" s="3"/>
     </row>
     <row r="10" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A10" s="1">
-        <v>3</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="H10" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" s="21" t="s">
-        <v>16</v>
-      </c>
+      <c r="A10" s="1"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
     </row>
     <row r="11" spans="1:16" customHeight="1" ht="21.9">
       <c r="A11" s="1"/>
@@ -1912,8 +1779,8 @@
   </sheetPr>
   <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0" zoomScale="115" zoomScaleNormal="115" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" workbookViewId="0" zoomScale="115" zoomScaleNormal="115" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1973,7 +1840,7 @@
     </row>
     <row r="5" spans="1:16" customHeight="1" ht="15.6">
       <c r="A5" s="17" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B5" s="17"/>
     </row>
@@ -2026,10 +1893,10 @@
         <v>1</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>15</v>
+        <v>23</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>18</v>
       </c>
       <c r="D8" s="21" t="s">
         <v>16</v>
@@ -2053,179 +1920,71 @@
       <c r="O8" s="4"/>
     </row>
     <row r="9" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A9" s="1">
-        <v>2</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="I9" s="21" t="s">
-        <v>16</v>
-      </c>
+      <c r="A9" s="1"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
       <c r="M9" s="3"/>
     </row>
     <row r="10" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A10" s="1">
-        <v>3</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="H10" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" s="21" t="s">
-        <v>16</v>
-      </c>
+      <c r="A10" s="1"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
     </row>
     <row r="11" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A11" s="1">
-        <v>4</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="I11" s="21" t="s">
-        <v>16</v>
-      </c>
+      <c r="A11" s="1"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
     </row>
     <row r="12" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A12" s="1">
-        <v>5</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="I12" s="21" t="s">
-        <v>16</v>
-      </c>
+      <c r="A12" s="1"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
     </row>
     <row r="13" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A13" s="1">
-        <v>6</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G13" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="H13" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="I13" s="21" t="s">
-        <v>16</v>
-      </c>
+      <c r="A13" s="1"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
     </row>
     <row r="14" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A14" s="1">
-        <v>7</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G14" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="H14" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="I14" s="21" t="s">
-        <v>16</v>
-      </c>
+      <c r="A14" s="1"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
     </row>
     <row r="15" spans="1:16" customHeight="1" ht="21.9">
       <c r="A15" s="1"/>
@@ -2248,722 +2007,6 @@
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
-    </row>
-    <row r="17" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A17" s="1"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-    </row>
-    <row r="18" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A18" s="1"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-    </row>
-    <row r="19" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A19" s="1"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-    </row>
-    <row r="20" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A20" s="1"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-    </row>
-    <row r="21" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A21" s="1"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-    </row>
-    <row r="22" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A22" s="1"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-    </row>
-    <row r="23" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A23" s="1"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-    </row>
-    <row r="24" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A24" s="1"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-    </row>
-    <row r="25" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A25" s="1"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
-    </row>
-    <row r="26" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A26" s="1"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
-    </row>
-    <row r="27" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A27" s="1"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-    </row>
-    <row r="28" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A28" s="1"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
-    </row>
-    <row r="29" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A29" s="1"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
-    </row>
-    <row r="30" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A30" s="1"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
-    </row>
-    <row r="31" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A31" s="1"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
-    </row>
-    <row r="32" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A32" s="1"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="9"/>
-    </row>
-    <row r="33" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A33" s="1"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
-    </row>
-    <row r="34" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A34" s="1"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="9"/>
-      <c r="I34" s="9"/>
-    </row>
-    <row r="35" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A35" s="1"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="9"/>
-    </row>
-    <row r="36" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A36" s="1"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
-      <c r="H36" s="9"/>
-      <c r="I36" s="9"/>
-    </row>
-    <row r="37" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A37" s="1"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
-      <c r="I37" s="9"/>
-    </row>
-    <row r="38" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A38" s="1"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
-      <c r="I38" s="9"/>
-    </row>
-    <row r="39" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A39" s="1"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
-      <c r="I39" s="9"/>
-    </row>
-    <row r="40" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A40" s="1"/>
-      <c r="B40" s="7"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="9"/>
-      <c r="G40" s="9"/>
-      <c r="H40" s="9"/>
-      <c r="I40" s="9"/>
-    </row>
-    <row r="41" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A41" s="1"/>
-      <c r="B41" s="7"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="9"/>
-      <c r="H41" s="9"/>
-      <c r="I41" s="9"/>
-    </row>
-    <row r="42" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A42" s="1"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="9"/>
-      <c r="H42" s="9"/>
-      <c r="I42" s="9"/>
-    </row>
-    <row r="43" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A43" s="1"/>
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="9"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="9"/>
-      <c r="H43" s="9"/>
-      <c r="I43" s="9"/>
-    </row>
-    <row r="44" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A44" s="2"/>
-      <c r="B44" s="11"/>
-      <c r="C44" s="11"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
-      <c r="G44" s="12"/>
-      <c r="H44" s="12"/>
-      <c r="I44" s="12"/>
-    </row>
-    <row r="45" spans="1:16" customHeight="1" ht="21.9"/>
-  </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <mergeCells>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A3:I3"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="D6:I6"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C6:C7"/>
-  </mergeCells>
-  <printOptions gridLines="false" gridLinesSet="true"/>
-  <pageMargins left="0.23622047244094" right="0.23622047244094" top="0.74803149606299" bottom="0.74803149606299" header="0.31496062992126" footer="0.31496062992126"/>
-  <pageSetup paperSize="9" orientation="portrait" scale="70" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" r:id="rId1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
-  <tableParts count="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
-  <dimension ref="A1:P45"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" zoomScale="115" zoomScaleNormal="115" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="I16" sqref="I16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col min="1" max="1" width="4" customWidth="true" style="0"/>
-    <col min="2" max="2" width="29.5546875" customWidth="true" style="0"/>
-    <col min="3" max="3" width="13.5546875" customWidth="true" style="0"/>
-    <col min="4" max="4" width="13.6640625" customWidth="true" style="0"/>
-    <col min="5" max="5" width="12.5546875" customWidth="true" style="0"/>
-    <col min="6" max="6" width="12.5546875" customWidth="true" style="0"/>
-    <col min="7" max="7" width="13" customWidth="true" style="0"/>
-    <col min="8" max="8" width="12.5546875" customWidth="true" style="0"/>
-    <col min="9" max="9" width="12.5546875" customWidth="true" style="0"/>
-    <col min="14" max="14" width="8.88671875" customWidth="true" style="0"/>
-    <col min="15" max="15" width="11.33203125" customWidth="true" style="0"/>
-    <col min="16" max="16" width="12.88671875" customWidth="true" style="0"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" customHeight="1" ht="18">
-      <c r="A1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-    </row>
-    <row r="2" spans="1:16" customHeight="1" ht="18">
-      <c r="A2" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-    </row>
-    <row r="3" spans="1:16" customHeight="1" ht="18">
-      <c r="A3" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-    </row>
-    <row r="5" spans="1:16" customHeight="1" ht="15.6">
-      <c r="A5" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="17"/>
-    </row>
-    <row r="6" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A6" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-    </row>
-    <row r="7" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A7" s="14"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-    </row>
-    <row r="8" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A8" s="1">
-        <v>1</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="N8" s="3"/>
-      <c r="O8" s="4"/>
-    </row>
-    <row r="9" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A9" s="1">
-        <v>2</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="I9" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="M9" s="3"/>
-    </row>
-    <row r="10" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A10" s="1">
-        <v>3</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="H10" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" s="21" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A11" s="1">
-        <v>4</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="I11" s="21" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A12" s="1">
-        <v>5</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="I12" s="21" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A13" s="1">
-        <v>6</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G13" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="H13" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="I13" s="21" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A14" s="1">
-        <v>7</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G14" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="H14" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="I14" s="21" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A15" s="1">
-        <v>8</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G15" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="H15" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="I15" s="21" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A16" s="1">
-        <v>9</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G16" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="H16" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="I16" s="21" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="17" spans="1:16" customHeight="1" ht="21.9">
       <c r="A17" s="1"/>

</xml_diff>

<commit_message>
update penggunaan kata Bahasa Indonesia
</commit_message>
<xml_diff>
--- a/public/template/Data Pembayaran Komite Semester Ganjil.xlsx
+++ b/public/template/Data Pembayaran Komite Semester Ganjil.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView activeTab="2" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView activeTab="3" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="27 jmy 6" sheetId="1" r:id="rId4"/>
-    <sheet name="12 MIA 2" sheetId="2" r:id="rId5"/>
-    <sheet name="04 gbk 2" sheetId="3" r:id="rId6"/>
+    <sheet name="X MIA 2" sheetId="1" r:id="rId4"/>
+    <sheet name="X IIS 3" sheetId="2" r:id="rId5"/>
+    <sheet name="XI IIS 2" sheetId="3" r:id="rId6"/>
+    <sheet name="12 MIA 2" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
@@ -17,18 +18,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="59">
   <si>
     <t>DAFTAR PEMBAYARAN ADMINISTRASI KOMITE</t>
   </si>
   <si>
-    <t>TAHUN AJARAN 20329</t>
+    <t>TAHUN AJARAN 2023/2024</t>
   </si>
   <si>
     <t>SEMESTER GANJIL (I)</t>
   </si>
   <si>
-    <t>KELAS 27 jmy 6</t>
+    <t>KELAS X MIA 2</t>
   </si>
   <si>
     <t>NO</t>
@@ -61,34 +62,139 @@
     <t>DESEMBER</t>
   </si>
   <si>
-    <t>Silvia Nurdiyanti</t>
+    <t>Diana Padmasari</t>
+  </si>
+  <si>
+    <t>Rp. 75.000</t>
+  </si>
+  <si>
+    <t>Belum Lunas</t>
+  </si>
+  <si>
+    <t>Saiful Sihotang</t>
+  </si>
+  <si>
+    <t>Cakrabirawa Narpati S.Ked</t>
+  </si>
+  <si>
+    <t>Wahyu Dongoran</t>
+  </si>
+  <si>
+    <t>Kamila Aryani</t>
+  </si>
+  <si>
+    <t>Zulaikha Zalindra Yuniar</t>
+  </si>
+  <si>
+    <t>Muhammad Natsir</t>
+  </si>
+  <si>
+    <t>Fitriani Mandasari</t>
+  </si>
+  <si>
+    <t>Jindra Parman Samosir</t>
+  </si>
+  <si>
+    <t>Kurnia Winarno</t>
+  </si>
+  <si>
+    <t>Ophelia Anggraini S.Pd</t>
+  </si>
+  <si>
+    <t>Junior Rakada</t>
+  </si>
+  <si>
+    <t>KELAS X IIS 3</t>
+  </si>
+  <si>
+    <t>Lantar Siregar S.H.</t>
+  </si>
+  <si>
+    <t>Prayoga Putra</t>
+  </si>
+  <si>
+    <t>Siska Kamilia</t>
+  </si>
+  <si>
+    <t>Dwi Marpaung S.Kom</t>
+  </si>
+  <si>
+    <t>Wani Farida S.Pt</t>
+  </si>
+  <si>
+    <t>Irnanto Sihombing S.Farm</t>
+  </si>
+  <si>
+    <t>Danu Anggriawan S.I.Kom</t>
+  </si>
+  <si>
+    <t>KELAS XI IIS 2</t>
+  </si>
+  <si>
+    <t>Tasdik Lazuardi</t>
+  </si>
+  <si>
+    <t>Kenari Darsirah Situmorang M.Kom.</t>
+  </si>
+  <si>
+    <t>Danang Wahyudin</t>
+  </si>
+  <si>
+    <t>Ibun Dongoran</t>
+  </si>
+  <si>
+    <t>Umaya Uwais</t>
+  </si>
+  <si>
+    <t>Violet Natalia Nasyiah</t>
+  </si>
+  <si>
+    <t>Atma Wibisono</t>
+  </si>
+  <si>
+    <t>Aslijan Wahyudin</t>
+  </si>
+  <si>
+    <t>Daru Thamrin</t>
+  </si>
+  <si>
+    <t>Kasiran Prasetya Firgantoro S.T.</t>
+  </si>
+  <si>
+    <t>KELAS 12 MIA 2</t>
+  </si>
+  <si>
+    <t>Sarah Agustina</t>
   </si>
   <si>
     <t>Rp. 0</t>
   </si>
   <si>
-    <t>Belum Lunas</t>
-  </si>
-  <si>
-    <t>Siska Genta Hasanah M.Ak</t>
-  </si>
-  <si>
-    <t>Rp. 420.000</t>
-  </si>
-  <si>
-    <t>Hudi Gloria</t>
-  </si>
-  <si>
-    <t>KELAS 12 MIA 2</t>
-  </si>
-  <si>
-    <t>Yosef Mustofa</t>
-  </si>
-  <si>
-    <t>KELAS 04 gbk 2</t>
-  </si>
-  <si>
-    <t>sadsads fe</t>
+    <t>Lunas</t>
+  </si>
+  <si>
+    <t>Lidya Puspasari</t>
+  </si>
+  <si>
+    <t>Kajen Karsana Hakim M.Ak</t>
+  </si>
+  <si>
+    <t>Pangestu Gunawan S.Farm</t>
+  </si>
+  <si>
+    <t>Ibun Bajragin Kuswoyo M.Ak</t>
+  </si>
+  <si>
+    <t>Dinda Utami</t>
+  </si>
+  <si>
+    <t>Kawaya Margana Hardiansyah</t>
+  </si>
+  <si>
+    <t>Eva Wastuti</t>
+  </si>
+  <si>
+    <t>Limar Sitompul</t>
   </si>
 </sst>
 </file>
@@ -151,13 +257,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF99CCFF"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FF99CCFF"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -600,7 +706,7 @@
   <dimension ref="A1:P45"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" zoomScale="115" zoomScaleNormal="115" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -718,22 +824,22 @@
       <c r="C8" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8" s="21" t="s">
+      <c r="D8" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="20" t="s">
         <v>16</v>
       </c>
       <c r="N8" s="3"/>
@@ -746,25 +852,25 @@
       <c r="B9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="I9" s="21" t="s">
+      <c r="C9" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="20" t="s">
         <v>16</v>
       </c>
       <c r="M9" s="3"/>
@@ -774,128 +880,290 @@
         <v>3</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" customHeight="1" ht="21.9">
+      <c r="A11" s="1">
+        <v>4</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="H10" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" s="21" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A11" s="1"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
+      <c r="C11" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="12" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A12" s="1"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
+      <c r="A12" s="1">
+        <v>5</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="13" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A13" s="1"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
+      <c r="A13" s="1">
+        <v>6</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" s="20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="14" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A14" s="1"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
+      <c r="A14" s="1">
+        <v>7</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" s="20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="15" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A15" s="1"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
+      <c r="A15" s="1">
+        <v>8</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I15" s="20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="16" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A16" s="1"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
+      <c r="A16" s="1">
+        <v>9</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="17" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A17" s="1"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
+      <c r="A17" s="1">
+        <v>10</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" s="20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="18" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A18" s="1"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
+      <c r="A18" s="1">
+        <v>11</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I18" s="20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="19" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A19" s="1"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
+      <c r="A19" s="1">
+        <v>12</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I19" s="20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="20" spans="1:16" customHeight="1" ht="21.9">
       <c r="A20" s="1"/>
@@ -1208,7 +1476,7 @@
   <dimension ref="A1:P45"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" zoomScale="115" zoomScaleNormal="115" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1268,7 +1536,7 @@
     </row>
     <row r="5" spans="1:16" customHeight="1" ht="15.6">
       <c r="A5" s="17" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B5" s="17"/>
     </row>
@@ -1321,98 +1589,206 @@
         <v>1</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="20" t="s">
         <v>16</v>
       </c>
       <c r="N8" s="3"/>
       <c r="O8" s="4"/>
     </row>
     <row r="9" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A9" s="1"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
+      <c r="A9" s="1">
+        <v>2</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>16</v>
+      </c>
       <c r="M9" s="3"/>
     </row>
     <row r="10" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A10" s="1"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
+      <c r="A10" s="1">
+        <v>3</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="11" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A11" s="1"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
+      <c r="A11" s="1">
+        <v>4</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="12" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A12" s="1"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
+      <c r="A12" s="1">
+        <v>5</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="13" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A13" s="1"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
+      <c r="A13" s="1">
+        <v>6</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" s="20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="14" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A14" s="1"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
+      <c r="A14" s="1">
+        <v>7</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" s="20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="15" spans="1:16" customHeight="1" ht="21.9">
       <c r="A15" s="1"/>
@@ -1779,8 +2155,8 @@
   </sheetPr>
   <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" zoomScale="115" zoomScaleNormal="115" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="0" workbookViewId="0" zoomScale="115" zoomScaleNormal="115" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1840,7 +2216,7 @@
     </row>
     <row r="5" spans="1:16" customHeight="1" ht="15.6">
       <c r="A5" s="17" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="B5" s="17"/>
     </row>
@@ -1893,120 +2269,998 @@
         <v>1</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="20" t="s">
         <v>16</v>
       </c>
       <c r="N8" s="3"/>
       <c r="O8" s="4"/>
     </row>
     <row r="9" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A9" s="1"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
+      <c r="A9" s="1">
+        <v>2</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>16</v>
+      </c>
       <c r="M9" s="3"/>
     </row>
     <row r="10" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A10" s="1"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
+      <c r="A10" s="1">
+        <v>3</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="11" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A11" s="1"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
+      <c r="A11" s="1">
+        <v>4</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="12" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A12" s="1"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
+      <c r="A12" s="1">
+        <v>5</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="13" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A13" s="1"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
+      <c r="A13" s="1">
+        <v>6</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" s="20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="14" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A14" s="1"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
+      <c r="A14" s="1">
+        <v>7</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" s="20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="15" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A15" s="1"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
+      <c r="A15" s="1">
+        <v>8</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I15" s="20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="16" spans="1:16" customHeight="1" ht="21.9">
-      <c r="A16" s="1"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
+      <c r="A16" s="1">
+        <v>9</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" customHeight="1" ht="21.9">
+      <c r="A17" s="1">
+        <v>10</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" s="20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" customHeight="1" ht="21.9">
+      <c r="A18" s="1"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+    </row>
+    <row r="19" spans="1:16" customHeight="1" ht="21.9">
+      <c r="A19" s="1"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+    </row>
+    <row r="20" spans="1:16" customHeight="1" ht="21.9">
+      <c r="A20" s="1"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+    </row>
+    <row r="21" spans="1:16" customHeight="1" ht="21.9">
+      <c r="A21" s="1"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+    </row>
+    <row r="22" spans="1:16" customHeight="1" ht="21.9">
+      <c r="A22" s="1"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+    </row>
+    <row r="23" spans="1:16" customHeight="1" ht="21.9">
+      <c r="A23" s="1"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+    </row>
+    <row r="24" spans="1:16" customHeight="1" ht="21.9">
+      <c r="A24" s="1"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+    </row>
+    <row r="25" spans="1:16" customHeight="1" ht="21.9">
+      <c r="A25" s="1"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+    </row>
+    <row r="26" spans="1:16" customHeight="1" ht="21.9">
+      <c r="A26" s="1"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+    </row>
+    <row r="27" spans="1:16" customHeight="1" ht="21.9">
+      <c r="A27" s="1"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+    </row>
+    <row r="28" spans="1:16" customHeight="1" ht="21.9">
+      <c r="A28" s="1"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+    </row>
+    <row r="29" spans="1:16" customHeight="1" ht="21.9">
+      <c r="A29" s="1"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+    </row>
+    <row r="30" spans="1:16" customHeight="1" ht="21.9">
+      <c r="A30" s="1"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+    </row>
+    <row r="31" spans="1:16" customHeight="1" ht="21.9">
+      <c r="A31" s="1"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+    </row>
+    <row r="32" spans="1:16" customHeight="1" ht="21.9">
+      <c r="A32" s="1"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+    </row>
+    <row r="33" spans="1:16" customHeight="1" ht="21.9">
+      <c r="A33" s="1"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+    </row>
+    <row r="34" spans="1:16" customHeight="1" ht="21.9">
+      <c r="A34" s="1"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+    </row>
+    <row r="35" spans="1:16" customHeight="1" ht="21.9">
+      <c r="A35" s="1"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
+    </row>
+    <row r="36" spans="1:16" customHeight="1" ht="21.9">
+      <c r="A36" s="1"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+    </row>
+    <row r="37" spans="1:16" customHeight="1" ht="21.9">
+      <c r="A37" s="1"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
+    </row>
+    <row r="38" spans="1:16" customHeight="1" ht="21.9">
+      <c r="A38" s="1"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
+    </row>
+    <row r="39" spans="1:16" customHeight="1" ht="21.9">
+      <c r="A39" s="1"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="9"/>
+    </row>
+    <row r="40" spans="1:16" customHeight="1" ht="21.9">
+      <c r="A40" s="1"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
+    </row>
+    <row r="41" spans="1:16" customHeight="1" ht="21.9">
+      <c r="A41" s="1"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="9"/>
+    </row>
+    <row r="42" spans="1:16" customHeight="1" ht="21.9">
+      <c r="A42" s="1"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
+      <c r="I42" s="9"/>
+    </row>
+    <row r="43" spans="1:16" customHeight="1" ht="21.9">
+      <c r="A43" s="1"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
+      <c r="I43" s="9"/>
+    </row>
+    <row r="44" spans="1:16" customHeight="1" ht="21.9">
+      <c r="A44" s="2"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="12"/>
+      <c r="I44" s="12"/>
+    </row>
+    <row r="45" spans="1:16" customHeight="1" ht="21.9"/>
+  </sheetData>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <mergeCells>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="D6:I6"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C6:C7"/>
+  </mergeCells>
+  <printOptions gridLines="false" gridLinesSet="true"/>
+  <pageMargins left="0.23622047244094" right="0.23622047244094" top="0.74803149606299" bottom="0.74803149606299" header="0.31496062992126" footer="0.31496062992126"/>
+  <pageSetup paperSize="9" orientation="portrait" scale="70" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" r:id="rId1"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+  <tableParts count="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:P45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0" zoomScale="115" zoomScaleNormal="115" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="4" customWidth="true" style="0"/>
+    <col min="2" max="2" width="29.5546875" customWidth="true" style="0"/>
+    <col min="3" max="3" width="13.5546875" customWidth="true" style="0"/>
+    <col min="4" max="4" width="13.6640625" customWidth="true" style="0"/>
+    <col min="5" max="5" width="12.5546875" customWidth="true" style="0"/>
+    <col min="6" max="6" width="12.5546875" customWidth="true" style="0"/>
+    <col min="7" max="7" width="13" customWidth="true" style="0"/>
+    <col min="8" max="8" width="12.5546875" customWidth="true" style="0"/>
+    <col min="9" max="9" width="12.5546875" customWidth="true" style="0"/>
+    <col min="14" max="14" width="8.88671875" customWidth="true" style="0"/>
+    <col min="15" max="15" width="11.33203125" customWidth="true" style="0"/>
+    <col min="16" max="16" width="12.88671875" customWidth="true" style="0"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" customHeight="1" ht="18">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+    </row>
+    <row r="2" spans="1:16" customHeight="1" ht="18">
+      <c r="A2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+    </row>
+    <row r="3" spans="1:16" customHeight="1" ht="18">
+      <c r="A3" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+    </row>
+    <row r="5" spans="1:16" customHeight="1" ht="15.6">
+      <c r="A5" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="17"/>
+    </row>
+    <row r="6" spans="1:16" customHeight="1" ht="21.9">
+      <c r="A6" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+    </row>
+    <row r="7" spans="1:16" customHeight="1" ht="21.9">
+      <c r="A7" s="14"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+    </row>
+    <row r="8" spans="1:16" customHeight="1" ht="21.9">
+      <c r="A8" s="1">
+        <v>1</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="N8" s="3"/>
+      <c r="O8" s="4"/>
+    </row>
+    <row r="9" spans="1:16" customHeight="1" ht="21.9">
+      <c r="A9" s="1">
+        <v>2</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="M9" s="3"/>
+    </row>
+    <row r="10" spans="1:16" customHeight="1" ht="21.9">
+      <c r="A10" s="1">
+        <v>3</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" customHeight="1" ht="21.9">
+      <c r="A11" s="1">
+        <v>4</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" customHeight="1" ht="21.9">
+      <c r="A12" s="1">
+        <v>5</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" customHeight="1" ht="21.9">
+      <c r="A13" s="1">
+        <v>6</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" s="20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" customHeight="1" ht="21.9">
+      <c r="A14" s="1">
+        <v>7</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" s="20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" customHeight="1" ht="21.9">
+      <c r="A15" s="1">
+        <v>8</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I15" s="20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" customHeight="1" ht="21.9">
+      <c r="A16" s="1">
+        <v>9</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="20" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="17" spans="1:16" customHeight="1" ht="21.9">
       <c r="A17" s="1"/>

</xml_diff>